<commit_message>
actualizacion de package raw_master
</commit_message>
<xml_diff>
--- a/Bitacora_Cargas.xlsx
+++ b/Bitacora_Cargas.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvaldes\Desktop\poc_cmf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F20995-A52A-4B5A-9FAF-ED26F61A5CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C519872E-5669-4B44-8CC8-B41125B5415A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1ACCDE6D-AFB0-413D-BDFE-14BC63DCB8CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1ACCDE6D-AFB0-413D-BDFE-14BC63DCB8CB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bitacora_cargas" sheetId="1" r:id="rId1"/>
-    <sheet name="Comandos" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="4" r:id="rId3"/>
+    <sheet name="Comandos" sheetId="2" r:id="rId1"/>
+    <sheet name="Bitacora de cargas" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>Nombre de la tabla</t>
   </si>
@@ -65,16 +64,10 @@
     <t>ok</t>
   </si>
   <si>
-    <t>tbl_poc_cmf_activosbanco2_mes</t>
-  </si>
-  <si>
     <t>Transaction</t>
   </si>
   <si>
     <t>Num_meses</t>
-  </si>
-  <si>
-    <t>tbl_poc_cmf_activosbanco1_mes</t>
   </si>
   <si>
     <t>tbl_poc_cmf_product_n1</t>
@@ -157,6 +150,45 @@
   </si>
   <si>
     <t>process_institucion</t>
+  </si>
+  <si>
+    <t>instituciones_cmf</t>
+  </si>
+  <si>
+    <t>process_productN1</t>
+  </si>
+  <si>
+    <t>process_productN2</t>
+  </si>
+  <si>
+    <t>process_productN3</t>
+  </si>
+  <si>
+    <t>process_productN4</t>
+  </si>
+  <si>
+    <t>process_productN5</t>
+  </si>
+  <si>
+    <t>process_product</t>
+  </si>
+  <si>
+    <t>Ejecutable</t>
+  </si>
+  <si>
+    <t>process_activosbanco1_mes</t>
+  </si>
+  <si>
+    <t>process_activosbanco2_mes</t>
+  </si>
+  <si>
+    <t>sudo -su hdfs spark-submit --master local --jars huemul-bigdatagovernance-2.6.2.jar,huemul-sql-decode-1.0.jar,poc_settings-2.6.2.jar,postgresql-9.4.1212.jar --class com.soluciones.poc_cmf.process_raw_master poc_cmf-2.6.2.jar environment=production,ano=2019,mes=09</t>
+  </si>
+  <si>
+    <t>sudo -su hdfs spark-submit --master local --jars huemul-bigdatagovernance-2.6.2.jar,huemul-sql-decode-1.0.jar,poc_settings-2.6.2.jar,postgresql-9.4.1212.jar --class com.soluciones.poc_cmf.process_raw_transaction poc_cmf-2.6.2.jar environment=production,ano=2019,mes=09,num_meses=4</t>
+  </si>
+  <si>
+    <t>sudo -su hdfs spark-submit --master local --jars huemul-bigdatagovernance-2.6.2.jar,huemul-sql-decode-1.0.jar,poc_settings-2.6.2.jar,postgresql-9.4.1212.jar --class com.soluciones.poc_cmf.process_raw_transaction poc_cmf-2.6.2.jar environment=production,ano=2020,mes=01,num_meses=9</t>
   </si>
 </sst>
 </file>
@@ -188,12 +220,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -201,6 +227,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,27 +329,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -327,7 +359,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,374 +684,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6D0EEE-E453-44DD-8E85-D3643F2792D1}">
-  <dimension ref="A2:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10">
-        <v>201909</v>
-      </c>
-      <c r="E10">
-        <v>201912</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>202001</v>
-      </c>
-      <c r="E11">
-        <v>202009</v>
-      </c>
-      <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>201909</v>
-      </c>
-      <c r="E12">
-        <v>201912</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>202001</v>
-      </c>
-      <c r="E13">
-        <v>202009</v>
-      </c>
-      <c r="F13">
-        <v>9</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>201909</v>
-      </c>
-      <c r="E14">
-        <v>201912</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>202001</v>
-      </c>
-      <c r="E15">
-        <v>202009</v>
-      </c>
-      <c r="F15">
-        <v>9</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8F7534-CB51-4CE2-A084-577E9403F6A3}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -1026,124 +701,124 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="16"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="16"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="16"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1156,12 +831,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70159B83-C2FA-4F5D-85F4-03E426B6B6E2}">
-  <dimension ref="B2:J11"/>
+  <dimension ref="B2:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,43 +846,47 @@
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1223,14 +902,23 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1246,20 +934,21 @@
         <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1275,17 +964,21 @@
         <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1301,17 +994,21 @@
         <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1327,17 +1024,21 @@
         <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="20"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1353,17 +1054,21 @@
         <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1379,21 +1084,25 @@
         <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="2:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>201909</v>
@@ -1405,18 +1114,24 @@
         <v>4</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
+      <c r="J10" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>202001</v>
@@ -1428,10 +1143,19 @@
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K3:K9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>